<commit_message>
xpaths added for cdp dashboard
xpaths added for cdp dashboard
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/Suite_Web.xlsx
+++ b/src/main/java/com/cdp/InputFiles/Suite_Web.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="75" yWindow="-15" windowWidth="20730" windowHeight="11760" tabRatio="626"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -507,7 +507,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Dashboard testcases added and Screen shots added in HTML reports
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/Suite_Web.xlsx
+++ b/src/main/java/com/cdp/InputFiles/Suite_Web.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="15210" windowHeight="6375" tabRatio="626"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="15210" windowHeight="4560" tabRatio="626"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>TSID</t>
   </si>
@@ -35,6 +35,15 @@
   </si>
   <si>
     <t>CDPDASHBOARD</t>
+  </si>
+  <si>
+    <t>DEFAULTDASHBOARD</t>
+  </si>
+  <si>
+    <t>ADDWIDGETS</t>
+  </si>
+  <si>
+    <t>REMOVEWIDGETS</t>
   </si>
 </sst>
 </file>
@@ -513,10 +522,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -556,6 +565,30 @@
       </c>
       <c r="B4" s="5" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>